<commit_message>
Fixing some minor bugs
</commit_message>
<xml_diff>
--- a/Decentralised CES/test_result/G bigger than D.xlsx
+++ b/Decentralised CES/test_result/G bigger than D.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">request!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -900,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>

</xml_diff>